<commit_message>
Clear notebook and move functions to modules
</commit_message>
<xml_diff>
--- a/dataset/dataset_1.xlsx
+++ b/dataset/dataset_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29103"/>
   <workbookPr date1904="1"/>
   <xr:revisionPtr revIDLastSave="0" documentId="11_288EEC2161B68AF7DB84C01E09B6800ACB2F6D53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
@@ -13,7 +13,7 @@
     <sheet name="D_lambda" sheetId="3" r:id="rId3"/>
     <sheet name="MmuE" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -416,15 +416,15 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,235 +786,235 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="8">
         <v>2</v>
       </c>
-      <c r="C1" s="10">
+      <c r="C1" s="8">
         <v>2</v>
       </c>
-      <c r="D1" s="10">
+      <c r="D1" s="8">
         <v>2</v>
       </c>
-      <c r="E1" s="10">
+      <c r="E1" s="8">
         <v>2</v>
       </c>
-      <c r="F1" s="10">
+      <c r="F1" s="8">
         <v>2</v>
       </c>
-      <c r="G1" s="10">
+      <c r="G1" s="8">
         <v>2</v>
       </c>
-      <c r="H1" s="10">
+      <c r="H1" s="8">
         <v>2</v>
       </c>
-      <c r="I1" s="10">
+      <c r="I1" s="8">
         <v>2</v>
       </c>
-      <c r="J1" s="10">
+      <c r="J1" s="8">
         <v>2</v>
       </c>
-      <c r="K1" s="10">
+      <c r="K1" s="8">
         <v>2</v>
       </c>
-      <c r="L1" s="10">
+      <c r="L1" s="8">
         <v>2</v>
       </c>
-      <c r="M1" s="11">
-        <v>1</v>
-      </c>
-      <c r="N1" s="11">
-        <v>1</v>
-      </c>
-      <c r="O1" s="11">
-        <v>1</v>
-      </c>
-      <c r="P1" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="12">
-        <v>3</v>
-      </c>
-      <c r="R1" s="12">
-        <v>3</v>
-      </c>
-      <c r="S1" s="12">
-        <v>3</v>
-      </c>
-      <c r="T1" s="12">
-        <v>3</v>
-      </c>
-      <c r="U1" s="12">
-        <v>3</v>
-      </c>
-      <c r="V1" s="12">
-        <v>3</v>
-      </c>
-      <c r="W1" s="12">
-        <v>3</v>
-      </c>
-      <c r="X1" s="12">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="12">
-        <v>3</v>
-      </c>
-      <c r="Z1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="10">
+      <c r="M1" s="9">
+        <v>1</v>
+      </c>
+      <c r="N1" s="9">
+        <v>1</v>
+      </c>
+      <c r="O1" s="9">
+        <v>1</v>
+      </c>
+      <c r="P1" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="10">
+        <v>3</v>
+      </c>
+      <c r="R1" s="10">
+        <v>3</v>
+      </c>
+      <c r="S1" s="10">
+        <v>3</v>
+      </c>
+      <c r="T1" s="10">
+        <v>3</v>
+      </c>
+      <c r="U1" s="10">
+        <v>3</v>
+      </c>
+      <c r="V1" s="10">
+        <v>3</v>
+      </c>
+      <c r="W1" s="10">
+        <v>3</v>
+      </c>
+      <c r="X1" s="10">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="10">
+        <v>3</v>
+      </c>
+      <c r="Z1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AA1" s="8">
         <v>2</v>
       </c>
-      <c r="AB1" s="10">
+      <c r="AB1" s="8">
         <v>2</v>
       </c>
-      <c r="AC1" s="10">
+      <c r="AC1" s="8">
         <v>2</v>
       </c>
-      <c r="AD1" s="10">
+      <c r="AD1" s="8">
         <v>2</v>
       </c>
-      <c r="AE1" s="10">
+      <c r="AE1" s="8">
         <v>2</v>
       </c>
-      <c r="AF1" s="10">
+      <c r="AF1" s="8">
         <v>2</v>
       </c>
-      <c r="AG1" s="10">
+      <c r="AG1" s="8">
         <v>2</v>
       </c>
-      <c r="AH1" s="10">
+      <c r="AH1" s="8">
         <v>2</v>
       </c>
-      <c r="AI1" s="10">
+      <c r="AI1" s="8">
         <v>2</v>
       </c>
-      <c r="AJ1" s="10">
+      <c r="AJ1" s="8">
         <v>2</v>
       </c>
-      <c r="AK1" s="10">
+      <c r="AK1" s="8">
         <v>2</v>
       </c>
-      <c r="AL1" s="11">
-        <v>1</v>
-      </c>
-      <c r="AM1" s="11">
-        <v>1</v>
-      </c>
-      <c r="AN1" s="11">
-        <v>1</v>
-      </c>
-      <c r="AO1" s="11">
-        <v>1</v>
-      </c>
-      <c r="AP1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AQ1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AR1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AS1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AT1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AU1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AV1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AW1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AX1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AY1" s="12">
-        <v>3</v>
-      </c>
-      <c r="AZ1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BA1" s="10">
+      <c r="AL1" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="9">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AQ1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AR1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AS1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AT1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AU1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AW1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AX1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AY1" s="10">
+        <v>3</v>
+      </c>
+      <c r="AZ1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BA1" s="8">
         <v>2</v>
       </c>
-      <c r="BB1" s="10">
+      <c r="BB1" s="8">
         <v>2</v>
       </c>
-      <c r="BC1" s="10">
+      <c r="BC1" s="8">
         <v>2</v>
       </c>
-      <c r="BD1" s="10">
+      <c r="BD1" s="8">
         <v>2</v>
       </c>
-      <c r="BE1" s="10">
+      <c r="BE1" s="8">
         <v>2</v>
       </c>
-      <c r="BF1" s="10">
+      <c r="BF1" s="8">
         <v>2</v>
       </c>
-      <c r="BG1" s="10">
+      <c r="BG1" s="8">
         <v>2</v>
       </c>
-      <c r="BH1" s="10">
+      <c r="BH1" s="8">
         <v>2</v>
       </c>
-      <c r="BI1" s="10">
+      <c r="BI1" s="8">
         <v>2</v>
       </c>
-      <c r="BJ1" s="10">
+      <c r="BJ1" s="8">
         <v>2</v>
       </c>
-      <c r="BK1" s="10">
+      <c r="BK1" s="8">
         <v>2</v>
       </c>
-      <c r="BL1" s="11">
-        <v>1</v>
-      </c>
-      <c r="BM1" s="11">
-        <v>1</v>
-      </c>
-      <c r="BN1" s="11">
-        <v>1</v>
-      </c>
-      <c r="BO1" s="11">
-        <v>1</v>
-      </c>
-      <c r="BP1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BQ1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BR1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BS1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BT1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BU1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BV1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BW1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BX1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BY1" s="12">
-        <v>3</v>
-      </c>
-      <c r="BZ1" s="12">
+      <c r="BL1" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM1" s="9">
+        <v>1</v>
+      </c>
+      <c r="BN1" s="9">
+        <v>1</v>
+      </c>
+      <c r="BO1" s="9">
+        <v>1</v>
+      </c>
+      <c r="BP1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BQ1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BR1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BS1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BT1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BU1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BV1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BW1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BX1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BY1" s="10">
+        <v>3</v>
+      </c>
+      <c r="BZ1" s="10">
         <v>3</v>
       </c>
     </row>
@@ -8477,19 +8477,19 @@
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>